<commit_message>
Added a few things in my part
</commit_message>
<xml_diff>
--- a/Entrega2/TabelaCompetencias.xlsx
+++ b/Entrega2/TabelaCompetencias.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="205" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="205"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="42">
   <si>
     <t>Competências Técnicas</t>
   </si>
@@ -41,7 +40,7 @@
     <t>Ana</t>
   </si>
   <si>
-    <t>C </t>
+    <t>C</t>
   </si>
   <si>
     <t>Avançado</t>
@@ -147,32 +146,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="6">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -192,247 +173,505 @@
     </fill>
   </fills>
   <borders count="11">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="hair"/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="hair"/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="hair"/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="hair"/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="hair"/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="hair"/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="18">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D53" activeCellId="0" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.76530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.48469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.43367346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.79081632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.48469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" width="9.7109375"/>
+    <col min="2" max="2" width="10.42578125"/>
+    <col min="3" max="3" width="9.42578125"/>
+    <col min="4" max="4" width="14.5703125"/>
+    <col min="5" max="5" width="6.42578125"/>
+    <col min="6" max="6" width="8.85546875"/>
+    <col min="7" max="7" width="9.42578125"/>
+    <col min="8" max="8" width="24.42578125"/>
+    <col min="9" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:8" ht="15.75">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:8" ht="14.25">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="1"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8">
       <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
@@ -453,7 +692,7 @@
       </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:8" ht="14.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -463,7 +702,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:8" ht="14.25">
       <c r="A5" s="11"/>
       <c r="B5" s="10" t="s">
         <v>8</v>
@@ -487,12 +726,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:8" ht="14.25">
       <c r="A6" s="11"/>
       <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -509,12 +748,12 @@
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:8" ht="14.25">
       <c r="A7" s="11"/>
       <c r="B7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="10"/>
@@ -527,12 +766,12 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:8">
       <c r="A8" s="13"/>
       <c r="B8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="10"/>
@@ -545,12 +784,12 @@
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:8">
       <c r="A9" s="13"/>
       <c r="B9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="10"/>
@@ -563,12 +802,12 @@
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:8">
       <c r="A10" s="13"/>
       <c r="B10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="10"/>
@@ -581,12 +820,12 @@
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:8">
       <c r="A11" s="13"/>
       <c r="B11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="10"/>
@@ -595,12 +834,12 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:8">
       <c r="A12" s="13"/>
       <c r="B12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="10"/>
@@ -609,12 +848,12 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:8">
       <c r="A13" s="13"/>
       <c r="B13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="10"/>
@@ -623,14 +862,14 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:8">
       <c r="A14" s="13"/>
       <c r="B14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="5"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:8" ht="14.25">
       <c r="A15" s="11" t="s">
         <v>29</v>
       </c>
@@ -639,7 +878,7 @@
       <c r="E15" s="5"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:8">
       <c r="A16" s="13"/>
       <c r="B16" s="10" t="s">
         <v>30</v>
@@ -655,7 +894,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:8">
       <c r="A17" s="13"/>
       <c r="B17" s="10" t="s">
         <v>8</v>
@@ -669,7 +908,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:8">
       <c r="A18" s="13"/>
       <c r="B18" s="10" t="s">
         <v>17</v>
@@ -683,7 +922,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:8">
       <c r="A19" s="13"/>
       <c r="B19" s="10" t="s">
         <v>27</v>
@@ -697,7 +936,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:8">
       <c r="A20" s="13"/>
       <c r="B20" s="10" t="s">
         <v>28</v>
@@ -709,7 +948,7 @@
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:8">
       <c r="A21" s="13"/>
       <c r="B21" s="10" t="s">
         <v>19</v>
@@ -721,7 +960,7 @@
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:8">
       <c r="A22" s="13"/>
       <c r="B22" s="10" t="s">
         <v>24</v>
@@ -730,7 +969,7 @@
       <c r="E22" s="5"/>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:8">
       <c r="A23" s="13"/>
       <c r="B23" s="10" t="s">
         <v>26</v>
@@ -739,7 +978,7 @@
       <c r="E23" s="5"/>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:8">
       <c r="A24" s="13"/>
       <c r="B24" s="10" t="s">
         <v>35</v>
@@ -748,21 +987,21 @@
       <c r="E24" s="5"/>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:8">
       <c r="A25" s="13"/>
       <c r="B25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="5"/>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:8">
       <c r="A26" s="13"/>
       <c r="B26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="5"/>
       <c r="H26" s="13"/>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:8" ht="14.25">
       <c r="A27" s="11" t="s">
         <v>36</v>
       </c>
@@ -771,7 +1010,7 @@
       <c r="E27" s="5"/>
       <c r="H27" s="13"/>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:8">
       <c r="A28" s="13"/>
       <c r="B28" s="10" t="s">
         <v>30</v>
@@ -787,7 +1026,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:8">
       <c r="A29" s="13"/>
       <c r="B29" s="10" t="s">
         <v>24</v>
@@ -799,7 +1038,7 @@
       </c>
       <c r="H29" s="13"/>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:8">
       <c r="A30" s="13"/>
       <c r="B30" s="10" t="s">
         <v>26</v>
@@ -811,7 +1050,7 @@
       </c>
       <c r="H30" s="13"/>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:8">
       <c r="A31" s="13"/>
       <c r="B31" s="10" t="s">
         <v>37</v>
@@ -823,12 +1062,12 @@
       </c>
       <c r="H31" s="13"/>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:8">
       <c r="A32" s="13"/>
       <c r="B32" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" t="s">
         <v>23</v>
       </c>
       <c r="D32" s="10"/>
@@ -838,7 +1077,7 @@
       </c>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:8">
       <c r="A33" s="13"/>
       <c r="B33" s="10" t="s">
         <v>27</v>
@@ -850,7 +1089,7 @@
       </c>
       <c r="H33" s="13"/>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:8">
       <c r="A34" s="13"/>
       <c r="B34" s="10" t="s">
         <v>28</v>
@@ -859,7 +1098,7 @@
       <c r="E34" s="5"/>
       <c r="H34" s="13"/>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:8">
       <c r="A35" s="13"/>
       <c r="B35" s="10" t="s">
         <v>38</v>
@@ -868,7 +1107,7 @@
       <c r="E35" s="5"/>
       <c r="H35" s="13"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:8">
       <c r="A36" s="13"/>
       <c r="B36" s="10" t="s">
         <v>39</v>
@@ -877,14 +1116,14 @@
       <c r="E36" s="5"/>
       <c r="H36" s="13"/>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:8">
       <c r="A37" s="13"/>
       <c r="B37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="5"/>
       <c r="H37" s="13"/>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:8" ht="14.25">
       <c r="A38" s="11" t="s">
         <v>40</v>
       </c>
@@ -893,7 +1132,7 @@
       <c r="E38" s="5"/>
       <c r="H38" s="13"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:8">
       <c r="A39" s="13"/>
       <c r="B39" s="10" t="s">
         <v>30</v>
@@ -905,38 +1144,56 @@
       <c r="F39" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="G39" s="18" t="s">
+        <v>23</v>
+      </c>
       <c r="H39" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:8">
       <c r="A40" s="13"/>
       <c r="B40" s="10" t="s">
         <v>24</v>
+      </c>
+      <c r="C40" t="s">
+        <v>23</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="5"/>
       <c r="F40" s="10" t="s">
         <v>16</v>
       </c>
+      <c r="G40" s="18" t="s">
+        <v>23</v>
+      </c>
       <c r="H40" s="13"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:8">
       <c r="A41" s="13"/>
       <c r="B41" s="10" t="s">
         <v>26</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="5"/>
       <c r="F41" s="10" t="s">
         <v>18</v>
       </c>
+      <c r="G41" s="18" t="s">
+        <v>23</v>
+      </c>
       <c r="H41" s="13"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:8">
       <c r="A42" s="13"/>
       <c r="B42" s="10" t="s">
         <v>37</v>
+      </c>
+      <c r="C42" t="s">
+        <v>23</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="5"/>
@@ -945,12 +1202,12 @@
       </c>
       <c r="H42" s="13"/>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:8">
       <c r="A43" s="13"/>
       <c r="B43" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" t="s">
         <v>23</v>
       </c>
       <c r="D43" s="10"/>
@@ -958,21 +1215,30 @@
       <c r="F43" s="10" t="s">
         <v>22</v>
       </c>
+      <c r="G43" s="18" t="s">
+        <v>11</v>
+      </c>
       <c r="H43" s="13"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:8">
       <c r="A44" s="13"/>
       <c r="B44" s="10" t="s">
         <v>27</v>
+      </c>
+      <c r="C44" t="s">
+        <v>23</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="5"/>
       <c r="F44" s="10" t="s">
         <v>25</v>
       </c>
+      <c r="G44" s="18" t="s">
+        <v>11</v>
+      </c>
       <c r="H44" s="13"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:8">
       <c r="A45" s="13"/>
       <c r="B45" s="10" t="s">
         <v>28</v>
@@ -981,21 +1247,26 @@
       <c r="E45" s="5"/>
       <c r="H45" s="13"/>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:8">
       <c r="A46" s="13"/>
       <c r="B46" s="10" t="s">
         <v>38</v>
       </c>
+      <c r="C46" t="s">
+        <v>23</v>
+      </c>
       <c r="D46" s="10"/>
       <c r="E46" s="5"/>
       <c r="H46" s="13"/>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:8">
       <c r="A47" s="14"/>
       <c r="B47" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="16"/>
+      <c r="C47" s="16" t="s">
+        <v>23</v>
+      </c>
       <c r="D47" s="15"/>
       <c r="E47" s="17"/>
       <c r="F47" s="16"/>
@@ -1009,10 +1280,9 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="90" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>